<commit_message>
easter adjustements to sync to vensim
</commit_message>
<xml_diff>
--- a/datafiles/initial_species.xlsx
+++ b/datafiles/initial_species.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdalm\AppData\Local\Terraformer2D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d641367ab90122e/_tec/codi/GM/Terraformer2D/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1B06B06-FD19-4F7C-87D3-C5413F848ED4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{D1B06B06-FD19-4F7C-87D3-C5413F848ED4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7D301DB5-E2CF-4D86-8196-8E8FE77F0FBF}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="285" windowWidth="21225" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="300" windowWidth="21225" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial_species" sheetId="3" r:id="rId1"/>
@@ -209,9 +209,6 @@
     <t>BIOMASS_ADULT</t>
   </si>
   <si>
-    <t>METABOLIC_RATE</t>
-  </si>
-  <si>
     <t>TEMPERATURE_OPTIMAL</t>
   </si>
   <si>
@@ -324,6 +321,9 @@
   </si>
   <si>
     <t>DEPRECATED_GROWTH_KG_YR</t>
+  </si>
+  <si>
+    <t>KC_METABOLIC_RATE</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -430,6 +430,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -443,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -466,6 +472,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -874,10 +883,10 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +896,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1">
         <v>2</v>
@@ -895,7 +904,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>8</v>
@@ -933,22 +942,22 @@
     </row>
     <row r="5" spans="1:12" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>12</v>
@@ -957,7 +966,7 @@
         <v>13</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>15</v>
@@ -1091,16 +1100,16 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" t="s">
         <v>17</v>
@@ -1109,7 +1118,7 @@
         <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J9" t="s">
         <v>19</v>
@@ -1148,7 +1157,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1267,7 +1276,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1433,7 +1442,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24">
         <v>0.4</v>
@@ -1485,7 +1494,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B26" s="1">
         <v>0.2</v>
@@ -1494,7 +1503,7 @@
         <v>0.2</v>
       </c>
       <c r="D26" s="1">
-        <v>0.2</v>
+        <v>0.09</v>
       </c>
       <c r="E26" s="1">
         <v>0.8</v>
@@ -1523,7 +1532,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="1">
         <v>30</v>
@@ -1561,7 +1570,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1">
         <v>15</v>
@@ -1569,8 +1578,8 @@
       <c r="C28" s="1">
         <v>5</v>
       </c>
-      <c r="D28" s="1">
-        <v>15</v>
+      <c r="D28" s="12">
+        <v>30</v>
       </c>
       <c r="E28" s="1">
         <v>10</v>
@@ -1599,36 +1608,36 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="1">
         <v>0.4</v>
       </c>
       <c r="C29" s="1">
-        <v>0.4</v>
+        <v>0.04</v>
       </c>
       <c r="D29" s="1">
-        <v>0.3</v>
+        <v>0.01</v>
       </c>
       <c r="E29" s="1">
-        <v>0.6</v>
+        <v>0.06</v>
       </c>
       <c r="F29" s="1">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="G29" s="1">
-        <v>0.4</v>
+        <v>0.04</v>
       </c>
       <c r="H29" s="1">
-        <v>0.4</v>
+        <v>0.04</v>
       </c>
       <c r="I29" s="1">
-        <v>0.4</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="1">
         <v>400</v>
@@ -1657,7 +1666,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" s="1">
         <v>1.2</v>
@@ -1686,7 +1695,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1">
         <v>50</v>
@@ -1715,7 +1724,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
@@ -1744,17 +1753,17 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -1775,16 +1784,16 @@
     </row>
     <row r="38" spans="1:12" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F38" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="F38" s="10" t="s">
+      <c r="I38" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -1797,36 +1806,36 @@
       </c>
       <c r="C41" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D41" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F41" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I41" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B42">
         <f>+B26</f>
@@ -1838,7 +1847,7 @@
       </c>
       <c r="D42">
         <f>+D26</f>
-        <v>0.2</v>
+        <v>0.09</v>
       </c>
       <c r="E42">
         <f>+E26</f>
@@ -1863,7 +1872,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43">
         <f>+B29*$B$1</f>
@@ -1871,36 +1880,36 @@
       </c>
       <c r="C43">
         <f>+C29*$B$1</f>
-        <v>0.8</v>
+        <v>0.08</v>
       </c>
       <c r="D43">
         <f>+D29*$B$1</f>
-        <v>0.6</v>
+        <v>0.02</v>
       </c>
       <c r="E43">
         <f>+E29*$B$1</f>
-        <v>1.2</v>
+        <v>0.12</v>
       </c>
       <c r="F43">
         <f t="shared" ref="F43:G43" si="3">+F29*$B$1</f>
-        <v>0.4</v>
+        <v>0.04</v>
       </c>
       <c r="G43">
         <f t="shared" si="3"/>
-        <v>0.8</v>
+        <v>0.08</v>
       </c>
       <c r="H43">
         <f t="shared" ref="H43:I43" si="4">+H29*$B$1</f>
-        <v>0.8</v>
+        <v>0.08</v>
       </c>
       <c r="I43">
         <f t="shared" si="4"/>
-        <v>0.8</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B44" s="6">
         <f>+B42/B43</f>
@@ -1908,31 +1917,31 @@
       </c>
       <c r="C44" s="6">
         <f>+C42/C43</f>
-        <v>0.25</v>
+        <v>2.5</v>
       </c>
       <c r="D44" s="6">
         <f>+D42/D43</f>
-        <v>0.33333333333333337</v>
+        <v>4.5</v>
       </c>
       <c r="E44" s="6">
         <f>+E42/E43</f>
-        <v>0.66666666666666674</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="F44" s="6">
         <f t="shared" ref="F44:G44" si="5">+F42/F43</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G44" s="6">
         <f t="shared" si="5"/>
-        <v>0.25</v>
+        <v>2.5</v>
       </c>
       <c r="H44" s="6">
         <f t="shared" ref="H44:I44" si="6">+H42/H43</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="I44" s="6">
         <f t="shared" si="6"/>
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2033,7 +2042,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2041,7 +2050,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -2089,7 +2098,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -2097,7 +2106,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -2105,7 +2114,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16">
         <v>11</v>
@@ -2113,7 +2122,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17">
         <v>12</v>
@@ -2121,7 +2130,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18">
         <v>13</v>
@@ -2129,7 +2138,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19">
         <v>14</v>
@@ -2137,7 +2146,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20">
         <v>15</v>
@@ -2145,7 +2154,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21">
         <v>99</v>

</xml_diff>

<commit_message>
adjusting morphology for plants with no trunk
</commit_message>
<xml_diff>
--- a/datafiles/initial_species.xlsx
+++ b/datafiles/initial_species.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d641367ab90122e/_tec/codi/GM/Terraformer2D/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{9828CACF-C433-4BD3-8EC2-D880FF0C148B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{64FAB9F3-1087-4B2B-91A3-C8DBC3C92DE5}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{9828CACF-C433-4BD3-8EC2-D880FF0C148B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AAAFBDA1-E8CE-4610-A902-A56A229F65C4}"/>
   <bookViews>
-    <workbookView xWindow="9150" yWindow="450" windowWidth="21225" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5805" yWindow="405" windowWidth="21225" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial_species" sheetId="3" r:id="rId1"/>
@@ -915,7 +915,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,25 +1818,25 @@
         <v>20</v>
       </c>
       <c r="C35" s="1">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D35" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E35" s="1">
         <v>50</v>
       </c>
       <c r="F35" s="1">
-        <v>0.5</v>
+        <v>30</v>
       </c>
       <c r="G35" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="H35" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I35" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
species color using blend and SPECIE_CUE gen
</commit_message>
<xml_diff>
--- a/datafiles/initial_species.xlsx
+++ b/datafiles/initial_species.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d641367ab90122e/_tec/codi/GM/Terraformer2D/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="8_{9828CACF-C433-4BD3-8EC2-D880FF0C148B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B3455BDB-88CD-4734-8F88-F8FA03E1FE3E}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="8_{9828CACF-C433-4BD3-8EC2-D880FF0C148B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8FA88DEA-BB65-4F11-BC5B-9325E0647CC5}"/>
   <bookViews>
     <workbookView xWindow="8355" yWindow="840" windowWidth="21225" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,9 +192,6 @@
     <t>PARENT_SPECIE_CODE</t>
   </si>
   <si>
-    <t>EMPTY5</t>
-  </si>
-  <si>
     <t>EMPTY6</t>
   </si>
   <si>
@@ -382,6 +379,9 @@
   </si>
   <si>
     <t>All gen value must be numeric - no empty cells</t>
+  </si>
+  <si>
+    <t>SPECIE_HUE</t>
   </si>
 </sst>
 </file>
@@ -961,7 +961,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J31" sqref="J31"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="B12:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,18 +971,18 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1">
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>8</v>
@@ -1020,22 +1020,22 @@
     </row>
     <row r="5" spans="1:12" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>12</v>
@@ -1044,7 +1044,7 @@
         <v>13</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>15</v>
@@ -1123,7 +1123,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2">
         <f>VLOOKUP(B5,Tabla1[#All],2,FALSE)</f>
@@ -1172,22 +1172,22 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" t="s">
         <v>17</v>
@@ -1196,7 +1196,7 @@
         <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J9" t="s">
         <v>19</v>
@@ -1210,7 +1210,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1286,45 +1286,45 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16">
         <v>12</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18">
         <v>64</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21">
         <v>800</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>0.1</v>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24">
         <v>0.4</v>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="1">
         <v>0.2</v>
@@ -1856,7 +1856,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="1">
         <v>30</v>
@@ -1894,7 +1894,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="1">
         <v>15</v>
@@ -1932,7 +1932,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" s="11">
         <v>0.9</v>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="1">
         <v>0.4</v>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1">
         <v>1600</v>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="1">
         <v>1.2</v>
@@ -2160,7 +2160,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="1">
         <v>100</v>
@@ -2198,7 +2198,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
@@ -2261,16 +2261,16 @@
     </row>
     <row r="41" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F41" s="7" t="s">
+      <c r="I41" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2312,7 +2312,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45">
         <f t="shared" ref="B45:I45" si="1">+B26</f>
@@ -2349,7 +2349,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46">
         <f t="shared" ref="B46:I46" si="2">+B32*$B$1</f>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" s="6">
         <f>+B45/B46</f>
@@ -2519,7 +2519,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2527,7 +2527,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -2583,7 +2583,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16">
         <v>11</v>
@@ -2599,7 +2599,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>12</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18">
         <v>13</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19">
         <v>14</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20">
         <v>15</v>
@@ -2631,7 +2631,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21">
         <v>99</v>
@@ -2690,21 +2690,21 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
         <v>85</v>
-      </c>
-      <c r="E1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3">
         <v>1.5</v>
@@ -2738,7 +2738,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4">
         <v>2.5</v>
@@ -2755,7 +2755,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5">
         <v>9999999</v>
@@ -2772,19 +2772,19 @@
     </row>
     <row r="10" spans="1:7" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>